<commit_message>
Se agrega modificacion para realizar deslogue y obtener los datos de prueba desde excel
</commit_message>
<xml_diff>
--- a/src/test/resources/pruebas_data_driven.xlsx
+++ b/src/test/resources/pruebas_data_driven.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\git\curso\curso-web-driver\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D997C06-30D1-4667-BC1E-277B5CFD5EA7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6585" xr2:uid="{1014A676-E1EB-4C79-84AB-0F97E53A0FD7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6585"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>PEPITO</t>
   </si>
@@ -39,12 +38,33 @@
   </si>
   <si>
     <t>CARDONA</t>
+  </si>
+  <si>
+    <t>PEPITO1</t>
+  </si>
+  <si>
+    <t>PEPITO2</t>
+  </si>
+  <si>
+    <t>PEPITO3</t>
+  </si>
+  <si>
+    <t>PEPITO4</t>
+  </si>
+  <si>
+    <t>PEPITO5</t>
+  </si>
+  <si>
+    <t>PEREZ2</t>
+  </si>
+  <si>
+    <t>PEREZ1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -389,11 +409,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D0173A-0BDC-4746-B70F-DECF7AF23537}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,6 +429,61 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>